<commit_message>
reordenación de archivos de Calc y Excel
</commit_message>
<xml_diff>
--- a/AGE(OPE2017)/EJERCICIOS/EXCEL 2010/00 archivos/10 - FUNCIONES MATEMÁTICAS/excel_fun_mat_05.xlsx
+++ b/AGE(OPE2017)/EJERCICIOS/EXCEL 2010/00 archivos/10 - FUNCIONES MATEMÁTICAS/excel_fun_mat_05.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Pedido</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>¿Cuántos pedidos se realizaron antes del 8/6/2010</t>
-  </si>
-  <si>
     <t>Raíz cuadrada</t>
   </si>
   <si>
@@ -52,10 +49,10 @@
     <t>Resto</t>
   </si>
   <si>
-    <t>Si para servir los kilos de nuestros pedidos usasemos sacos de 25 Kg, cuántos sacos harían falta para servir los pedidos del día 14?</t>
-  </si>
-  <si>
-    <t>Importe de los pedidos anteriores</t>
+    <t>Si para servir los kilos de nuestros pedidos usásemos sacos de 25 Kg, cuántos sacos harían falta para servir los pedidos del día 14?</t>
+  </si>
+  <si>
+    <t>Importe de los pedidos anteriores al 8/6/2018</t>
   </si>
 </sst>
 </file>
@@ -129,11 +126,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +435,7 @@
   <dimension ref="A3:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,9 +469,9 @@
         <v>1</v>
       </c>
       <c r="B4" s="4">
-        <v>40331</v>
-      </c>
-      <c r="C4" s="11">
+        <v>43253</v>
+      </c>
+      <c r="C4" s="10">
         <v>1004</v>
       </c>
       <c r="D4" s="1">
@@ -488,9 +485,9 @@
         <v>2</v>
       </c>
       <c r="B5" s="4">
-        <v>40332</v>
-      </c>
-      <c r="C5" s="11">
+        <v>43254</v>
+      </c>
+      <c r="C5" s="10">
         <v>1092</v>
       </c>
       <c r="D5" s="1">
@@ -504,9 +501,9 @@
         <v>3</v>
       </c>
       <c r="B6" s="4">
-        <v>40333</v>
-      </c>
-      <c r="C6" s="11">
+        <v>43255</v>
+      </c>
+      <c r="C6" s="10">
         <v>1128</v>
       </c>
       <c r="D6" s="1">
@@ -520,9 +517,9 @@
         <v>4</v>
       </c>
       <c r="B7" s="4">
-        <v>40336</v>
-      </c>
-      <c r="C7" s="11">
+        <v>43256</v>
+      </c>
+      <c r="C7" s="10">
         <v>1157</v>
       </c>
       <c r="D7" s="1">
@@ -536,9 +533,9 @@
         <v>5</v>
       </c>
       <c r="B8" s="4">
-        <v>40337</v>
-      </c>
-      <c r="C8" s="11">
+        <v>43257</v>
+      </c>
+      <c r="C8" s="10">
         <v>1360</v>
       </c>
       <c r="D8" s="1">
@@ -552,9 +549,9 @@
         <v>6</v>
       </c>
       <c r="B9" s="4">
-        <v>40338</v>
-      </c>
-      <c r="C9" s="11">
+        <v>43258</v>
+      </c>
+      <c r="C9" s="10">
         <v>1189</v>
       </c>
       <c r="D9" s="1">
@@ -568,9 +565,9 @@
         <v>7</v>
       </c>
       <c r="B10" s="4">
-        <v>40339</v>
-      </c>
-      <c r="C10" s="11">
+        <v>43259</v>
+      </c>
+      <c r="C10" s="10">
         <v>1084</v>
       </c>
       <c r="D10" s="1">
@@ -584,9 +581,9 @@
         <v>8</v>
       </c>
       <c r="B11" s="4">
-        <v>40340</v>
-      </c>
-      <c r="C11" s="11">
+        <v>43260</v>
+      </c>
+      <c r="C11" s="10">
         <v>1349</v>
       </c>
       <c r="D11" s="1">
@@ -601,9 +598,9 @@
         <v>9</v>
       </c>
       <c r="B12" s="4">
-        <v>40343</v>
-      </c>
-      <c r="C12" s="11">
+        <v>43261</v>
+      </c>
+      <c r="C12" s="10">
         <v>1391</v>
       </c>
       <c r="D12" s="1">
@@ -617,9 +614,9 @@
         <v>10</v>
       </c>
       <c r="B13" s="4">
-        <v>40344</v>
-      </c>
-      <c r="C13" s="11">
+        <v>43262</v>
+      </c>
+      <c r="C13" s="10">
         <v>1308</v>
       </c>
       <c r="D13" s="1">
@@ -663,22 +660,20 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="A19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="8"/>
       <c r="F19" s="1"/>
     </row>
@@ -692,9 +687,9 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="B21" s="9"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -702,9 +697,9 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="10"/>
+        <v>8</v>
+      </c>
+      <c r="B22" s="9"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -712,9 +707,9 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="10"/>
+        <v>9</v>
+      </c>
+      <c r="B23" s="9"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -722,9 +717,9 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="10"/>
+        <v>10</v>
+      </c>
+      <c r="B24" s="9"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -732,11 +727,11 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
+      <c r="B27" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
archivos Calc y Excel
</commit_message>
<xml_diff>
--- a/AGE(OPE2017)/EJERCICIOS/EXCEL 2010/00 archivos/10 - FUNCIONES MATEMÁTICAS/excel_fun_mat_05.xlsx
+++ b/AGE(OPE2017)/EJERCICIOS/EXCEL 2010/00 archivos/10 - FUNCIONES MATEMÁTICAS/excel_fun_mat_05.xlsx
@@ -49,10 +49,10 @@
     <t>Resto</t>
   </si>
   <si>
-    <t>Si para servir los kilos de nuestros pedidos usásemos sacos de 25 Kg, cuántos sacos harían falta para servir los pedidos del día 14?</t>
-  </si>
-  <si>
     <t>Importe de los pedidos anteriores al 8/6/2018</t>
+  </si>
+  <si>
+    <t>Si para servir los kilos de nuestros pedidos usásemos sacos de 25 Kg, ¿cuántos sacos harían falta para servir los pedidos del día 10?</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A3:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +669,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -727,7 +727,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>